<commit_message>
Feat: VGG19 model using Transfer learning
Accuracy: 72.37%
</commit_message>
<xml_diff>
--- a/Udacity/Artificial Intelligence Nanodegree/Dog Breed Detection Using CNN/TransferLearningStudy.xlsx
+++ b/Udacity/Artificial Intelligence Nanodegree/Dog Breed Detection Using CNN/TransferLearningStudy.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="VGG16" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="VGG19" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t xml:space="preserve">VGG 16 </t>
   </si>
@@ -64,13 +64,25 @@
   </si>
   <si>
     <t>with 2 additional layer</t>
+  </si>
+  <si>
+    <t>VGG19</t>
+  </si>
+  <si>
+    <t>Relu</t>
+  </si>
+  <si>
+    <t>softmax</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +93,18 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
@@ -104,15 +128,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,20 +448,20 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="H1" s="1" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
@@ -505,7 +536,7 @@
       <c r="B10">
         <v>20</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>0.49641099999999999</v>
       </c>
     </row>
@@ -516,10 +547,10 @@
       <c r="B11">
         <v>20</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>0.59689000000000003</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>0.61124400000000001</v>
       </c>
     </row>
@@ -530,7 +561,7 @@
       <c r="B12">
         <v>20</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>0.59330099999999997</v>
       </c>
     </row>
@@ -541,7 +572,7 @@
       <c r="B13">
         <v>20</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>0.53588499999999994</v>
       </c>
     </row>
@@ -552,7 +583,7 @@
       <c r="B14">
         <v>40</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>0.60645899999999997</v>
       </c>
     </row>
@@ -563,7 +594,7 @@
       <c r="B15">
         <v>50</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>0.55263200000000001</v>
       </c>
     </row>
@@ -574,7 +605,7 @@
       <c r="B16">
         <v>40</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>0.631579</v>
       </c>
     </row>
@@ -585,7 +616,7 @@
       <c r="B17">
         <v>40</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>0.59210499999999999</v>
       </c>
     </row>
@@ -596,7 +627,7 @@
       <c r="B18">
         <v>100</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>0.61722500000000002</v>
       </c>
     </row>
@@ -607,7 +638,7 @@
       <c r="B19">
         <v>100</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>0.72129200000000004</v>
       </c>
       <c r="D19" t="s">
@@ -621,7 +652,7 @@
       <c r="B20">
         <v>100</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>0.71172199999999997</v>
       </c>
       <c r="D20" t="s">
@@ -641,7 +672,7 @@
       <c r="B21">
         <v>50</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>0.71650700000000001</v>
       </c>
       <c r="D21" t="s">
@@ -661,7 +692,7 @@
       <c r="B22">
         <v>100</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>0.72009599999999996</v>
       </c>
       <c r="D22" t="s">
@@ -675,22 +706,22 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23">
+      <c r="A23" s="5">
         <v>500</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="5">
         <v>100</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="6">
         <v>0.72368399999999999</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="5">
         <v>512</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="5">
         <v>256</v>
       </c>
     </row>
@@ -705,13 +736,258 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="H1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>256</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>133</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.71411500000000006</v>
+      </c>
+      <c r="D11" s="4">
+        <v>69.378</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.70693799999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>80</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.68301400000000001</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>200</v>
+      </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.73445000000000005</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>150</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.72727299999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>150</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.72129200000000004</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>300</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.70574199999999998</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>200</v>
+      </c>
+      <c r="B18">
+        <v>80</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.70813400000000004</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>200</v>
+      </c>
+      <c r="B21">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.703349</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="5">
+        <v>200</v>
+      </c>
+      <c r="B22" s="5">
+        <v>20</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.72129200000000004</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="5">
+        <v>512</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>